<commit_message>
added ProgessBar and Thread
</commit_message>
<xml_diff>
--- a/TestWithBash/ExcelTest2.xlsx
+++ b/TestWithBash/ExcelTest2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t xml:space="preserve">Ergebnis: </t>
   </si>
@@ -129,6 +129,183 @@
   </si>
   <si>
     <t>31.1.2013</t>
+  </si>
+  <si>
+    <t>1.2.2013</t>
+  </si>
+  <si>
+    <t>2.2.2013</t>
+  </si>
+  <si>
+    <t>3.2.2013</t>
+  </si>
+  <si>
+    <t>4.2.2013</t>
+  </si>
+  <si>
+    <t>5.2.2013</t>
+  </si>
+  <si>
+    <t>6.2.2013</t>
+  </si>
+  <si>
+    <t>7.2.2013</t>
+  </si>
+  <si>
+    <t>8.2.2013</t>
+  </si>
+  <si>
+    <t>9.2.2013</t>
+  </si>
+  <si>
+    <t>10.2.2013</t>
+  </si>
+  <si>
+    <t>11.2.2013</t>
+  </si>
+  <si>
+    <t>12.2.2013</t>
+  </si>
+  <si>
+    <t>13.2.2013</t>
+  </si>
+  <si>
+    <t>14.2.2013</t>
+  </si>
+  <si>
+    <t>15.2.2013</t>
+  </si>
+  <si>
+    <t>16.2.2013</t>
+  </si>
+  <si>
+    <t>17.2.2013</t>
+  </si>
+  <si>
+    <t>18.2.2013</t>
+  </si>
+  <si>
+    <t>19.2.2013</t>
+  </si>
+  <si>
+    <t>20.2.2013</t>
+  </si>
+  <si>
+    <t>21.2.2013</t>
+  </si>
+  <si>
+    <t>22.2.2013</t>
+  </si>
+  <si>
+    <t>23.2.2013</t>
+  </si>
+  <si>
+    <t>24.2.2013</t>
+  </si>
+  <si>
+    <t>25.2.2013</t>
+  </si>
+  <si>
+    <t>26.2.2013</t>
+  </si>
+  <si>
+    <t>27.2.2013</t>
+  </si>
+  <si>
+    <t>28.2.2013</t>
+  </si>
+  <si>
+    <t>1.3.2013</t>
+  </si>
+  <si>
+    <t>2.3.2013</t>
+  </si>
+  <si>
+    <t>3.3.2013</t>
+  </si>
+  <si>
+    <t>4.3.2013</t>
+  </si>
+  <si>
+    <t>5.3.2013</t>
+  </si>
+  <si>
+    <t>6.3.2013</t>
+  </si>
+  <si>
+    <t>7.3.2013</t>
+  </si>
+  <si>
+    <t>8.3.2013</t>
+  </si>
+  <si>
+    <t>9.3.2013</t>
+  </si>
+  <si>
+    <t>10.3.2013</t>
+  </si>
+  <si>
+    <t>11.3.2013</t>
+  </si>
+  <si>
+    <t>12.3.2013</t>
+  </si>
+  <si>
+    <t>13.3.2013</t>
+  </si>
+  <si>
+    <t>14.3.2013</t>
+  </si>
+  <si>
+    <t>15.3.2013</t>
+  </si>
+  <si>
+    <t>16.3.2013</t>
+  </si>
+  <si>
+    <t>17.3.2013</t>
+  </si>
+  <si>
+    <t>18.3.2013</t>
+  </si>
+  <si>
+    <t>19.3.2013</t>
+  </si>
+  <si>
+    <t>20.3.2013</t>
+  </si>
+  <si>
+    <t>21.3.2013</t>
+  </si>
+  <si>
+    <t>22.3.2013</t>
+  </si>
+  <si>
+    <t>23.3.2013</t>
+  </si>
+  <si>
+    <t>24.3.2013</t>
+  </si>
+  <si>
+    <t>25.3.2013</t>
+  </si>
+  <si>
+    <t>26.3.2013</t>
+  </si>
+  <si>
+    <t>27.3.2013</t>
+  </si>
+  <si>
+    <t>28.3.2013</t>
+  </si>
+  <si>
+    <t>29.3.2013</t>
+  </si>
+  <si>
+    <t>30.3.2013</t>
+  </si>
+  <si>
+    <t>31.3.2013</t>
   </si>
 </sst>
 </file>
@@ -218,13 +395,13 @@
         <v>0.0</v>
       </c>
       <c r="D3" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E3" t="n">
         <v>24.0</v>
       </c>
-      <c r="E3" t="n">
-        <v>27.0</v>
-      </c>
       <c r="F3" t="n">
-        <v>68.0</v>
+        <v>66.0</v>
       </c>
     </row>
     <row r="4">
@@ -244,7 +421,7 @@
         <v>34.0</v>
       </c>
       <c r="F4" t="n">
-        <v>76.0</v>
+        <v>74.0</v>
       </c>
     </row>
     <row r="5">
@@ -258,13 +435,13 @@
         <v>0.0</v>
       </c>
       <c r="D5" t="n">
-        <v>25.0</v>
+        <v>28.0</v>
       </c>
       <c r="E5" t="n">
-        <v>40.0</v>
+        <v>35.0</v>
       </c>
       <c r="F5" t="n">
-        <v>65.0</v>
+        <v>71.0</v>
       </c>
     </row>
     <row r="6">
@@ -278,13 +455,13 @@
         <v>0.0</v>
       </c>
       <c r="D6" t="n">
-        <v>29.0</v>
+        <v>25.0</v>
       </c>
       <c r="E6" t="n">
-        <v>33.0</v>
+        <v>30.0</v>
       </c>
       <c r="F6" t="n">
-        <v>79.0</v>
+        <v>71.0</v>
       </c>
     </row>
     <row r="7">
@@ -298,13 +475,13 @@
         <v>0.0</v>
       </c>
       <c r="D7" t="n">
-        <v>32.0</v>
+        <v>31.0</v>
       </c>
       <c r="E7" t="n">
-        <v>33.0</v>
+        <v>35.0</v>
       </c>
       <c r="F7" t="n">
-        <v>84.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="8">
@@ -318,13 +495,13 @@
         <v>0.0</v>
       </c>
       <c r="D8" t="n">
-        <v>31.0</v>
+        <v>26.0</v>
       </c>
       <c r="E8" t="n">
         <v>36.0</v>
       </c>
       <c r="F8" t="n">
-        <v>84.0</v>
+        <v>77.0</v>
       </c>
     </row>
     <row r="9">
@@ -338,10 +515,10 @@
         <v>0.0</v>
       </c>
       <c r="D9" t="n">
-        <v>24.0</v>
+        <v>21.0</v>
       </c>
       <c r="E9" t="n">
-        <v>46.0</v>
+        <v>54.0</v>
       </c>
       <c r="F9" t="n">
         <v>78.0</v>
@@ -358,13 +535,13 @@
         <v>0.0</v>
       </c>
       <c r="D10" t="n">
-        <v>29.0</v>
+        <v>24.0</v>
       </c>
       <c r="E10" t="n">
-        <v>43.0</v>
+        <v>42.0</v>
       </c>
       <c r="F10" t="n">
-        <v>84.0</v>
+        <v>79.0</v>
       </c>
     </row>
     <row r="11">
@@ -378,13 +555,13 @@
         <v>0.0</v>
       </c>
       <c r="D11" t="n">
-        <v>29.0</v>
+        <v>23.0</v>
       </c>
       <c r="E11" t="n">
-        <v>40.0</v>
+        <v>41.0</v>
       </c>
       <c r="F11" t="n">
-        <v>77.0</v>
+        <v>81.0</v>
       </c>
       <c r="G11" t="n">
         <v>20.0</v>
@@ -401,13 +578,13 @@
         <v>0.0</v>
       </c>
       <c r="D12" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="E12" t="n">
-        <v>39.0</v>
+        <v>36.0</v>
       </c>
       <c r="F12" t="n">
-        <v>75.0</v>
+        <v>77.0</v>
       </c>
     </row>
     <row r="13">
@@ -421,13 +598,13 @@
         <v>0.0</v>
       </c>
       <c r="D13" t="n">
-        <v>24.0</v>
+        <v>22.0</v>
       </c>
       <c r="E13" t="n">
-        <v>37.0</v>
+        <v>39.0</v>
       </c>
       <c r="F13" t="n">
-        <v>74.0</v>
+        <v>72.0</v>
       </c>
       <c r="G13" t="n">
         <v>-10.0</v>
@@ -444,13 +621,13 @@
         <v>0.0</v>
       </c>
       <c r="D14" t="n">
-        <v>28.0</v>
+        <v>30.0</v>
       </c>
       <c r="E14" t="n">
-        <v>29.0</v>
+        <v>26.0</v>
       </c>
       <c r="F14" t="n">
-        <v>79.0</v>
+        <v>68.0</v>
       </c>
     </row>
     <row r="15">
@@ -464,13 +641,13 @@
         <v>0.0</v>
       </c>
       <c r="D15" t="n">
-        <v>32.0</v>
+        <v>26.0</v>
       </c>
       <c r="E15" t="n">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="F15" t="n">
-        <v>69.0</v>
+        <v>72.0</v>
       </c>
     </row>
     <row r="16">
@@ -484,13 +661,13 @@
         <v>0.0</v>
       </c>
       <c r="D16" t="n">
-        <v>22.0</v>
+        <v>24.0</v>
       </c>
       <c r="E16" t="n">
-        <v>48.0</v>
+        <v>45.0</v>
       </c>
       <c r="F16" t="n">
-        <v>81.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="17">
@@ -504,13 +681,13 @@
         <v>0.0</v>
       </c>
       <c r="D17" t="n">
-        <v>22.0</v>
+        <v>24.0</v>
       </c>
       <c r="E17" t="n">
-        <v>41.0</v>
+        <v>37.0</v>
       </c>
       <c r="F17" t="n">
-        <v>74.0</v>
+        <v>77.0</v>
       </c>
     </row>
     <row r="18">
@@ -524,13 +701,13 @@
         <v>0.0</v>
       </c>
       <c r="D18" t="n">
-        <v>17.0</v>
+        <v>20.0</v>
       </c>
       <c r="E18" t="n">
-        <v>39.0</v>
+        <v>38.0</v>
       </c>
       <c r="F18" t="n">
-        <v>78.0</v>
+        <v>79.0</v>
       </c>
     </row>
     <row r="19">
@@ -544,13 +721,13 @@
         <v>0.0</v>
       </c>
       <c r="D19" t="n">
-        <v>22.0</v>
+        <v>20.0</v>
       </c>
       <c r="E19" t="n">
-        <v>36.0</v>
+        <v>41.0</v>
       </c>
       <c r="F19" t="n">
-        <v>75.0</v>
+        <v>71.0</v>
       </c>
     </row>
     <row r="20">
@@ -558,19 +735,19 @@
         <v>25</v>
       </c>
       <c r="B20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C20" t="n">
         <v>0.0</v>
       </c>
       <c r="D20" t="n">
-        <v>22.0</v>
+        <v>24.0</v>
       </c>
       <c r="E20" t="n">
-        <v>41.0</v>
+        <v>38.0</v>
       </c>
       <c r="F20" t="n">
-        <v>80.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="21">
@@ -584,13 +761,13 @@
         <v>0.0</v>
       </c>
       <c r="D21" t="n">
-        <v>27.0</v>
+        <v>22.0</v>
       </c>
       <c r="E21" t="n">
-        <v>34.0</v>
+        <v>32.0</v>
       </c>
       <c r="F21" t="n">
-        <v>71.0</v>
+        <v>68.0</v>
       </c>
     </row>
     <row r="22">
@@ -604,13 +781,13 @@
         <v>0.0</v>
       </c>
       <c r="D22" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="E22" t="n">
         <v>28.0</v>
       </c>
-      <c r="E22" t="n">
-        <v>31.0</v>
-      </c>
       <c r="F22" t="n">
-        <v>78.0</v>
+        <v>74.0</v>
       </c>
     </row>
     <row r="23">
@@ -627,10 +804,10 @@
         <v>26.0</v>
       </c>
       <c r="E23" t="n">
-        <v>38.0</v>
+        <v>44.0</v>
       </c>
       <c r="F23" t="n">
-        <v>74.0</v>
+        <v>68.0</v>
       </c>
     </row>
     <row r="24">
@@ -647,10 +824,10 @@
         <v>26.0</v>
       </c>
       <c r="E24" t="n">
-        <v>39.0</v>
+        <v>38.0</v>
       </c>
       <c r="F24" t="n">
-        <v>92.0</v>
+        <v>87.0</v>
       </c>
     </row>
     <row r="25">
@@ -664,7 +841,7 @@
         <v>0.0</v>
       </c>
       <c r="D25" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
       <c r="E25" t="n">
         <v>41.0</v>
@@ -684,16 +861,13 @@
         <v>0.0</v>
       </c>
       <c r="D26" t="n">
-        <v>19.0</v>
+        <v>28.0</v>
       </c>
       <c r="E26" t="n">
-        <v>41.0</v>
+        <v>36.0</v>
       </c>
       <c r="F26" t="n">
-        <v>90.0</v>
-      </c>
-      <c r="G26" t="n">
-        <v>50.0</v>
+        <v>87.0</v>
       </c>
     </row>
     <row r="27">
@@ -707,10 +881,10 @@
         <v>0.0</v>
       </c>
       <c r="D27" t="n">
-        <v>29.0</v>
+        <v>22.0</v>
       </c>
       <c r="E27" t="n">
-        <v>31.0</v>
+        <v>34.0</v>
       </c>
       <c r="F27" t="n">
         <v>79.0</v>
@@ -727,13 +901,13 @@
         <v>0.0</v>
       </c>
       <c r="D28" t="n">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="E28" t="n">
-        <v>26.0</v>
+        <v>30.0</v>
       </c>
       <c r="F28" t="n">
-        <v>92.0</v>
+        <v>84.0</v>
       </c>
     </row>
     <row r="29">
@@ -747,10 +921,10 @@
         <v>0.0</v>
       </c>
       <c r="D29" t="n">
-        <v>30.0</v>
+        <v>26.0</v>
       </c>
       <c r="E29" t="n">
-        <v>38.0</v>
+        <v>37.0</v>
       </c>
       <c r="F29" t="n">
         <v>73.0</v>
@@ -767,13 +941,13 @@
         <v>0.0</v>
       </c>
       <c r="D30" t="n">
-        <v>24.0</v>
+        <v>22.0</v>
       </c>
       <c r="E30" t="n">
-        <v>36.0</v>
+        <v>42.0</v>
       </c>
       <c r="F30" t="n">
-        <v>85.0</v>
+        <v>82.0</v>
       </c>
     </row>
     <row r="31">
@@ -787,10 +961,10 @@
         <v>0.0</v>
       </c>
       <c r="D31" t="n">
-        <v>29.0</v>
+        <v>25.0</v>
       </c>
       <c r="E31" t="n">
-        <v>40.0</v>
+        <v>36.0</v>
       </c>
       <c r="F31" t="n">
         <v>100.0</v>
@@ -807,10 +981,10 @@
         <v>0.0</v>
       </c>
       <c r="D32" t="n">
-        <v>32.0</v>
+        <v>29.0</v>
       </c>
       <c r="E32" t="n">
-        <v>46.0</v>
+        <v>42.0</v>
       </c>
       <c r="F32" t="n">
         <v>92.0</v>
@@ -827,13 +1001,1196 @@
         <v>0.0</v>
       </c>
       <c r="D33" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="E33" t="n">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
       <c r="F33" t="n">
         <v>88.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>95.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>89.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>91.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>97.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>94.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>92.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>77.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>88.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>92.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>87.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>93.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>84.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>81.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>81.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>93.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D53" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>92.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>99.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>87.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>93.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>92.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>83.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D62" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>89.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>73.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D65" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="E65" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>93.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D67" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>84.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D68" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D69" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="E71" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>88.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>87.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D73" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>93.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D75" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>89.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D76" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>81.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>96.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>83.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D81" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="E81" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>95.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D82" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="E82" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D83" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="E83" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>84.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D84" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="E84" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>77.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D85" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="E85" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="G85" t="n">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>86.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="F87" t="n">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D88" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="E88" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="F88" t="n">
+        <v>82.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>94</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D89" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="E89" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="F89" t="n">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>95</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D90" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E90" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>82.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>74.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>97</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="F92" t="n">
+        <v>72.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added null value to product data
</commit_message>
<xml_diff>
--- a/TestWithBash/ExcelTest2.xlsx
+++ b/TestWithBash/ExcelTest2.xlsx
@@ -20,16 +20,16 @@
     <t>Datum</t>
   </si>
   <si>
-    <t>neumann(-0.596)</t>
-  </si>
-  <si>
-    <t>mikrofon(0.997)</t>
-  </si>
-  <si>
-    <t>nickel(-0.693)</t>
-  </si>
-  <si>
-    <t>k87(NaN)</t>
+    <t>neumann(0.167)</t>
+  </si>
+  <si>
+    <t>mikrofon(0.133)</t>
+  </si>
+  <si>
+    <t>nickel(0.002)</t>
+  </si>
+  <si>
+    <t>k87(-0.015)</t>
   </si>
   <si>
     <t>K87 Kapsel(NaN)</t>
@@ -389,13 +389,13 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="C3" t="n">
-        <v>25.0</v>
+        <v>24.0</v>
       </c>
       <c r="D3" t="n">
-        <v>62.0</v>
+        <v>68.0</v>
       </c>
       <c r="E3" t="n">
         <v>0.0</v>
@@ -409,13 +409,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>29.0</v>
+        <v>34.0</v>
       </c>
       <c r="C4" t="n">
-        <v>22.0</v>
+        <v>30.0</v>
       </c>
       <c r="D4" t="n">
-        <v>67.0</v>
+        <v>76.0</v>
       </c>
       <c r="E4" t="n">
         <v>0.0</v>
@@ -429,13 +429,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>36.0</v>
+        <v>39.0</v>
       </c>
       <c r="C5" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="D5" t="n">
-        <v>63.0</v>
+        <v>71.0</v>
       </c>
       <c r="E5" t="n">
         <v>0.0</v>
@@ -449,13 +449,13 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>31.0</v>
+        <v>33.0</v>
       </c>
       <c r="C6" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="D6" t="n">
-        <v>71.0</v>
+        <v>76.0</v>
       </c>
       <c r="E6" t="n">
         <v>0.0</v>
@@ -469,13 +469,13 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="C7" t="n">
-        <v>26.0</v>
+        <v>29.0</v>
       </c>
       <c r="D7" t="n">
-        <v>70.0</v>
+        <v>77.0</v>
       </c>
       <c r="E7" t="n">
         <v>0.0</v>
@@ -489,13 +489,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>32.0</v>
+        <v>33.0</v>
       </c>
       <c r="C8" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="D8" t="n">
-        <v>66.0</v>
+        <v>79.0</v>
       </c>
       <c r="E8" t="n">
         <v>0.0</v>
@@ -509,13 +509,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>48.0</v>
+        <v>43.0</v>
       </c>
       <c r="C9" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="D9" t="n">
-        <v>80.0</v>
+        <v>81.0</v>
       </c>
       <c r="E9" t="n">
         <v>0.0</v>
@@ -529,13 +529,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>41.0</v>
+        <v>51.0</v>
       </c>
       <c r="C10" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
       <c r="D10" t="n">
-        <v>75.0</v>
+        <v>79.0</v>
       </c>
       <c r="E10" t="n">
         <v>0.0</v>
@@ -549,13 +549,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>38.0</v>
+        <v>42.0</v>
       </c>
       <c r="C11" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="D11" t="n">
-        <v>75.0</v>
+        <v>80.0</v>
       </c>
       <c r="E11" t="n">
         <v>0.0</v>
@@ -564,7 +564,7 @@
         <v>0.0</v>
       </c>
       <c r="G11" t="n">
-        <v>50.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="12">
@@ -572,18 +572,21 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>34.0</v>
+        <v>36.0</v>
       </c>
       <c r="C12" t="n">
-        <v>22.0</v>
+        <v>29.0</v>
       </c>
       <c r="D12" t="n">
-        <v>65.0</v>
+        <v>76.0</v>
       </c>
       <c r="E12" t="n">
         <v>0.0</v>
       </c>
       <c r="F12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -592,18 +595,21 @@
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>32.0</v>
+        <v>39.0</v>
       </c>
       <c r="C13" t="n">
-        <v>22.0</v>
+        <v>27.0</v>
       </c>
       <c r="D13" t="n">
-        <v>67.0</v>
+        <v>77.0</v>
       </c>
       <c r="E13" t="n">
         <v>0.0</v>
       </c>
       <c r="F13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -612,18 +618,21 @@
         <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="C14" t="n">
-        <v>24.0</v>
+        <v>30.0</v>
       </c>
       <c r="D14" t="n">
-        <v>76.0</v>
+        <v>77.0</v>
       </c>
       <c r="E14" t="n">
         <v>0.0</v>
       </c>
       <c r="F14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -632,18 +641,21 @@
         <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>33.0</v>
+        <v>36.0</v>
       </c>
       <c r="C15" t="n">
-        <v>27.0</v>
+        <v>37.0</v>
       </c>
       <c r="D15" t="n">
-        <v>67.0</v>
+        <v>74.0</v>
       </c>
       <c r="E15" t="n">
         <v>0.0</v>
       </c>
       <c r="F15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -652,18 +664,21 @@
         <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>45.0</v>
+        <v>51.0</v>
       </c>
       <c r="C16" t="n">
-        <v>22.0</v>
+        <v>24.0</v>
       </c>
       <c r="D16" t="n">
-        <v>65.0</v>
+        <v>78.0</v>
       </c>
       <c r="E16" t="n">
         <v>0.0</v>
       </c>
       <c r="F16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G16" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -672,18 +687,21 @@
         <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>39.0</v>
+        <v>44.0</v>
       </c>
       <c r="C17" t="n">
-        <v>24.0</v>
+        <v>26.0</v>
       </c>
       <c r="D17" t="n">
-        <v>69.0</v>
+        <v>76.0</v>
       </c>
       <c r="E17" t="n">
         <v>0.0</v>
       </c>
       <c r="F17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G17" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -692,18 +710,21 @@
         <v>23</v>
       </c>
       <c r="B18" t="n">
-        <v>33.0</v>
+        <v>39.0</v>
       </c>
       <c r="C18" t="n">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="D18" t="n">
-        <v>73.0</v>
+        <v>82.0</v>
       </c>
       <c r="E18" t="n">
         <v>0.0</v>
       </c>
       <c r="F18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G18" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -712,18 +733,21 @@
         <v>24</v>
       </c>
       <c r="B19" t="n">
-        <v>41.0</v>
+        <v>40.0</v>
       </c>
       <c r="C19" t="n">
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
       <c r="D19" t="n">
-        <v>71.0</v>
+        <v>75.0</v>
       </c>
       <c r="E19" t="n">
         <v>0.0</v>
       </c>
       <c r="F19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G19" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -732,18 +756,21 @@
         <v>25</v>
       </c>
       <c r="B20" t="n">
-        <v>35.0</v>
+        <v>41.0</v>
       </c>
       <c r="C20" t="n">
-        <v>22.0</v>
+        <v>25.0</v>
       </c>
       <c r="D20" t="n">
-        <v>71.0</v>
+        <v>82.0</v>
       </c>
       <c r="E20" t="n">
         <v>0.0</v>
       </c>
       <c r="F20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G20" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -752,18 +779,21 @@
         <v>26</v>
       </c>
       <c r="B21" t="n">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
       <c r="C21" t="n">
-        <v>23.0</v>
+        <v>29.0</v>
       </c>
       <c r="D21" t="n">
-        <v>66.0</v>
+        <v>73.0</v>
       </c>
       <c r="E21" t="n">
         <v>0.0</v>
       </c>
       <c r="F21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G21" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -772,18 +802,21 @@
         <v>27</v>
       </c>
       <c r="B22" t="n">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
       <c r="C22" t="n">
-        <v>21.0</v>
+        <v>29.0</v>
       </c>
       <c r="D22" t="n">
-        <v>72.0</v>
+        <v>80.0</v>
       </c>
       <c r="E22" t="n">
         <v>0.0</v>
       </c>
       <c r="F22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G22" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -792,18 +825,21 @@
         <v>28</v>
       </c>
       <c r="B23" t="n">
-        <v>32.0</v>
+        <v>44.0</v>
       </c>
       <c r="C23" t="n">
         <v>21.0</v>
       </c>
       <c r="D23" t="n">
-        <v>73.0</v>
+        <v>80.0</v>
       </c>
       <c r="E23" t="n">
         <v>0.0</v>
       </c>
       <c r="F23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G23" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -812,18 +848,21 @@
         <v>29</v>
       </c>
       <c r="B24" t="n">
-        <v>37.0</v>
+        <v>39.0</v>
       </c>
       <c r="C24" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="D24" t="n">
-        <v>78.0</v>
+        <v>95.0</v>
       </c>
       <c r="E24" t="n">
         <v>0.0</v>
       </c>
       <c r="F24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G24" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -832,18 +871,21 @@
         <v>30</v>
       </c>
       <c r="B25" t="n">
-        <v>35.0</v>
+        <v>39.0</v>
       </c>
       <c r="C25" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="D25" t="n">
-        <v>76.0</v>
+        <v>89.0</v>
       </c>
       <c r="E25" t="n">
         <v>0.0</v>
       </c>
       <c r="F25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G25" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -852,18 +894,21 @@
         <v>31</v>
       </c>
       <c r="B26" t="n">
-        <v>36.0</v>
+        <v>39.0</v>
       </c>
       <c r="C26" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="D26" t="n">
-        <v>83.0</v>
+        <v>95.0</v>
       </c>
       <c r="E26" t="n">
         <v>0.0</v>
       </c>
       <c r="F26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G26" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -872,18 +917,21 @@
         <v>32</v>
       </c>
       <c r="B27" t="n">
-        <v>30.0</v>
+        <v>33.0</v>
       </c>
       <c r="C27" t="n">
-        <v>20.0</v>
+        <v>28.0</v>
       </c>
       <c r="D27" t="n">
-        <v>75.0</v>
+        <v>86.0</v>
       </c>
       <c r="E27" t="n">
         <v>0.0</v>
       </c>
       <c r="F27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G27" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -892,18 +940,21 @@
         <v>33</v>
       </c>
       <c r="B28" t="n">
-        <v>32.0</v>
+        <v>30.0</v>
       </c>
       <c r="C28" t="n">
-        <v>26.0</v>
+        <v>28.0</v>
       </c>
       <c r="D28" t="n">
-        <v>80.0</v>
+        <v>89.0</v>
       </c>
       <c r="E28" t="n">
         <v>0.0</v>
       </c>
       <c r="F28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G28" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -912,18 +963,21 @@
         <v>34</v>
       </c>
       <c r="B29" t="n">
-        <v>31.0</v>
+        <v>35.0</v>
       </c>
       <c r="C29" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="D29" t="n">
-        <v>69.0</v>
+        <v>82.0</v>
       </c>
       <c r="E29" t="n">
         <v>0.0</v>
       </c>
       <c r="F29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G29" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -932,18 +986,21 @@
         <v>35</v>
       </c>
       <c r="B30" t="n">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
       <c r="C30" t="n">
-        <v>18.0</v>
+        <v>22.0</v>
       </c>
       <c r="D30" t="n">
-        <v>80.0</v>
+        <v>82.0</v>
       </c>
       <c r="E30" t="n">
         <v>0.0</v>
       </c>
       <c r="F30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G30" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -952,10 +1009,10 @@
         <v>36</v>
       </c>
       <c r="B31" t="n">
-        <v>36.0</v>
+        <v>34.0</v>
       </c>
       <c r="C31" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="D31" t="n">
         <v>100.0</v>
@@ -964,6 +1021,9 @@
         <v>0.0</v>
       </c>
       <c r="F31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G31" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -972,18 +1032,21 @@
         <v>37</v>
       </c>
       <c r="B32" t="n">
-        <v>37.0</v>
+        <v>43.0</v>
       </c>
       <c r="C32" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="D32" t="n">
-        <v>79.0</v>
+        <v>95.0</v>
       </c>
       <c r="E32" t="n">
         <v>0.0</v>
       </c>
       <c r="F32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G32" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -992,18 +1055,21 @@
         <v>38</v>
       </c>
       <c r="B33" t="n">
-        <v>35.0</v>
+        <v>46.0</v>
       </c>
       <c r="C33" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="D33" t="n">
-        <v>80.0</v>
+        <v>89.0</v>
       </c>
       <c r="E33" t="n">
         <v>0.0</v>
       </c>
       <c r="F33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G33" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1012,18 +1078,21 @@
         <v>39</v>
       </c>
       <c r="B34" t="n">
-        <v>41.0</v>
+        <v>45.0</v>
       </c>
       <c r="C34" t="n">
-        <v>25.0</v>
+        <v>22.0</v>
       </c>
       <c r="D34" t="n">
-        <v>86.0</v>
+        <v>91.0</v>
       </c>
       <c r="E34" t="n">
         <v>0.0</v>
       </c>
       <c r="F34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G34" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1032,18 +1101,21 @@
         <v>40</v>
       </c>
       <c r="B35" t="n">
-        <v>29.0</v>
+        <v>27.0</v>
       </c>
       <c r="C35" t="n">
-        <v>26.0</v>
+        <v>24.0</v>
       </c>
       <c r="D35" t="n">
-        <v>87.0</v>
+        <v>77.0</v>
       </c>
       <c r="E35" t="n">
         <v>0.0</v>
       </c>
       <c r="F35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G35" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1052,18 +1124,21 @@
         <v>41</v>
       </c>
       <c r="B36" t="n">
-        <v>28.0</v>
+        <v>30.0</v>
       </c>
       <c r="C36" t="n">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
       <c r="D36" t="n">
-        <v>90.0</v>
+        <v>83.0</v>
       </c>
       <c r="E36" t="n">
         <v>0.0</v>
       </c>
       <c r="F36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G36" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1072,18 +1147,21 @@
         <v>42</v>
       </c>
       <c r="B37" t="n">
-        <v>43.0</v>
+        <v>35.0</v>
       </c>
       <c r="C37" t="n">
-        <v>31.0</v>
+        <v>26.0</v>
       </c>
       <c r="D37" t="n">
-        <v>93.0</v>
+        <v>88.0</v>
       </c>
       <c r="E37" t="n">
         <v>0.0</v>
       </c>
       <c r="F37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G37" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1092,18 +1170,21 @@
         <v>43</v>
       </c>
       <c r="B38" t="n">
-        <v>40.0</v>
+        <v>37.0</v>
       </c>
       <c r="C38" t="n">
-        <v>26.0</v>
+        <v>28.0</v>
       </c>
       <c r="D38" t="n">
-        <v>94.0</v>
+        <v>91.0</v>
       </c>
       <c r="E38" t="n">
         <v>1.0</v>
       </c>
       <c r="F38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G38" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1112,18 +1193,21 @@
         <v>44</v>
       </c>
       <c r="B39" t="n">
-        <v>38.0</v>
+        <v>39.0</v>
       </c>
       <c r="C39" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="D39" t="n">
-        <v>100.0</v>
+        <v>90.0</v>
       </c>
       <c r="E39" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G39" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1135,15 +1219,18 @@
         <v>41.0</v>
       </c>
       <c r="C40" t="n">
-        <v>21.0</v>
+        <v>25.0</v>
       </c>
       <c r="D40" t="n">
-        <v>85.0</v>
+        <v>86.0</v>
       </c>
       <c r="E40" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G40" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1152,18 +1239,21 @@
         <v>46</v>
       </c>
       <c r="B41" t="n">
-        <v>38.0</v>
+        <v>34.0</v>
       </c>
       <c r="C41" t="n">
-        <v>22.0</v>
+        <v>27.0</v>
       </c>
       <c r="D41" t="n">
-        <v>91.0</v>
+        <v>90.0</v>
       </c>
       <c r="E41" t="n">
         <v>0.0</v>
       </c>
       <c r="F41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G41" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1172,10 +1262,10 @@
         <v>47</v>
       </c>
       <c r="B42" t="n">
-        <v>39.0</v>
+        <v>32.0</v>
       </c>
       <c r="C42" t="n">
-        <v>36.0</v>
+        <v>31.0</v>
       </c>
       <c r="D42" t="n">
         <v>82.0</v>
@@ -1184,6 +1274,9 @@
         <v>0.0</v>
       </c>
       <c r="F42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G42" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1192,18 +1285,21 @@
         <v>48</v>
       </c>
       <c r="B43" t="n">
-        <v>40.0</v>
+        <v>29.0</v>
       </c>
       <c r="C43" t="n">
         <v>27.0</v>
       </c>
       <c r="D43" t="n">
-        <v>82.0</v>
+        <v>84.0</v>
       </c>
       <c r="E43" t="n">
         <v>0.0</v>
       </c>
       <c r="F43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G43" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1212,13 +1308,13 @@
         <v>49</v>
       </c>
       <c r="B44" t="n">
-        <v>43.0</v>
+        <v>40.0</v>
       </c>
       <c r="C44" t="n">
-        <v>23.0</v>
+        <v>21.0</v>
       </c>
       <c r="D44" t="n">
-        <v>96.0</v>
+        <v>83.0</v>
       </c>
       <c r="E44" t="n">
         <v>0.0</v>
@@ -1227,7 +1323,7 @@
         <v>0.0</v>
       </c>
       <c r="G44" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="45">
@@ -1235,18 +1331,21 @@
         <v>50</v>
       </c>
       <c r="B45" t="n">
-        <v>46.0</v>
+        <v>45.0</v>
       </c>
       <c r="C45" t="n">
-        <v>29.0</v>
+        <v>23.0</v>
       </c>
       <c r="D45" t="n">
-        <v>93.0</v>
+        <v>100.0</v>
       </c>
       <c r="E45" t="n">
         <v>0.0</v>
       </c>
       <c r="F45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G45" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1255,18 +1354,21 @@
         <v>51</v>
       </c>
       <c r="B46" t="n">
-        <v>62.0</v>
+        <v>59.0</v>
       </c>
       <c r="C46" t="n">
-        <v>25.0</v>
+        <v>24.0</v>
       </c>
       <c r="D46" t="n">
-        <v>93.0</v>
+        <v>86.0</v>
       </c>
       <c r="E46" t="n">
         <v>0.0</v>
       </c>
       <c r="F46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G46" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1275,18 +1377,21 @@
         <v>52</v>
       </c>
       <c r="B47" t="n">
-        <v>49.0</v>
+        <v>39.0</v>
       </c>
       <c r="C47" t="n">
-        <v>23.0</v>
+        <v>26.0</v>
       </c>
       <c r="D47" t="n">
-        <v>96.0</v>
+        <v>82.0</v>
       </c>
       <c r="E47" t="n">
         <v>0.0</v>
       </c>
       <c r="F47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G47" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1295,18 +1400,21 @@
         <v>53</v>
       </c>
       <c r="B48" t="n">
-        <v>36.0</v>
+        <v>32.0</v>
       </c>
       <c r="C48" t="n">
-        <v>25.0</v>
+        <v>21.0</v>
       </c>
       <c r="D48" t="n">
-        <v>87.0</v>
+        <v>78.0</v>
       </c>
       <c r="E48" t="n">
         <v>0.0</v>
       </c>
       <c r="F48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G48" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1321,12 +1429,15 @@
         <v>30.0</v>
       </c>
       <c r="D49" t="n">
-        <v>81.0</v>
+        <v>79.0</v>
       </c>
       <c r="E49" t="n">
         <v>0.0</v>
       </c>
       <c r="F49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G49" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1335,18 +1446,21 @@
         <v>55</v>
       </c>
       <c r="B50" t="n">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
       <c r="C50" t="n">
-        <v>26.0</v>
+        <v>22.0</v>
       </c>
       <c r="D50" t="n">
-        <v>79.0</v>
+        <v>72.0</v>
       </c>
       <c r="E50" t="n">
         <v>0.0</v>
       </c>
       <c r="F50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G50" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1355,18 +1469,21 @@
         <v>56</v>
       </c>
       <c r="B51" t="n">
-        <v>39.0</v>
+        <v>45.0</v>
       </c>
       <c r="C51" t="n">
-        <v>28.0</v>
+        <v>25.0</v>
       </c>
       <c r="D51" t="n">
-        <v>92.0</v>
+        <v>91.0</v>
       </c>
       <c r="E51" t="n">
         <v>0.0</v>
       </c>
       <c r="F51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G51" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1375,10 +1492,10 @@
         <v>57</v>
       </c>
       <c r="B52" t="n">
-        <v>54.0</v>
+        <v>42.0</v>
       </c>
       <c r="C52" t="n">
-        <v>31.0</v>
+        <v>24.0</v>
       </c>
       <c r="D52" t="n">
         <v>92.0</v>
@@ -1387,6 +1504,9 @@
         <v>0.0</v>
       </c>
       <c r="F52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G52" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1395,18 +1515,21 @@
         <v>58</v>
       </c>
       <c r="B53" t="n">
-        <v>42.0</v>
+        <v>38.0</v>
       </c>
       <c r="C53" t="n">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="D53" t="n">
-        <v>92.0</v>
+        <v>86.0</v>
       </c>
       <c r="E53" t="n">
         <v>0.0</v>
       </c>
       <c r="F53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G53" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1415,18 +1538,21 @@
         <v>59</v>
       </c>
       <c r="B54" t="n">
-        <v>44.0</v>
+        <v>39.0</v>
       </c>
       <c r="C54" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="D54" t="n">
-        <v>97.0</v>
+        <v>94.0</v>
       </c>
       <c r="E54" t="n">
         <v>0.0</v>
       </c>
       <c r="F54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G54" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1435,10 +1561,10 @@
         <v>60</v>
       </c>
       <c r="B55" t="n">
-        <v>35.0</v>
+        <v>34.0</v>
       </c>
       <c r="C55" t="n">
-        <v>27.0</v>
+        <v>22.0</v>
       </c>
       <c r="D55" t="n">
         <v>89.0</v>
@@ -1447,6 +1573,9 @@
         <v>0.0</v>
       </c>
       <c r="F55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G55" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1455,18 +1584,21 @@
         <v>61</v>
       </c>
       <c r="B56" t="n">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
       <c r="C56" t="n">
-        <v>30.0</v>
+        <v>24.0</v>
       </c>
       <c r="D56" t="n">
-        <v>82.0</v>
+        <v>87.0</v>
       </c>
       <c r="E56" t="n">
         <v>0.0</v>
       </c>
       <c r="F56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G56" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1475,18 +1607,21 @@
         <v>62</v>
       </c>
       <c r="B57" t="n">
-        <v>33.0</v>
+        <v>31.0</v>
       </c>
       <c r="C57" t="n">
-        <v>30.0</v>
+        <v>26.0</v>
       </c>
       <c r="D57" t="n">
-        <v>80.0</v>
+        <v>79.0</v>
       </c>
       <c r="E57" t="n">
         <v>0.0</v>
       </c>
       <c r="F57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G57" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1495,18 +1630,21 @@
         <v>63</v>
       </c>
       <c r="B58" t="n">
-        <v>37.0</v>
+        <v>35.0</v>
       </c>
       <c r="C58" t="n">
-        <v>26.0</v>
+        <v>20.0</v>
       </c>
       <c r="D58" t="n">
-        <v>86.0</v>
+        <v>80.0</v>
       </c>
       <c r="E58" t="n">
         <v>0.0</v>
       </c>
       <c r="F58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G58" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1515,18 +1653,21 @@
         <v>64</v>
       </c>
       <c r="B59" t="n">
-        <v>48.0</v>
+        <v>36.0</v>
       </c>
       <c r="C59" t="n">
-        <v>27.0</v>
+        <v>22.0</v>
       </c>
       <c r="D59" t="n">
-        <v>98.0</v>
+        <v>81.0</v>
       </c>
       <c r="E59" t="n">
         <v>0.0</v>
       </c>
       <c r="F59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G59" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1535,18 +1676,21 @@
         <v>65</v>
       </c>
       <c r="B60" t="n">
-        <v>50.0</v>
+        <v>43.0</v>
       </c>
       <c r="C60" t="n">
-        <v>26.0</v>
+        <v>21.0</v>
       </c>
       <c r="D60" t="n">
-        <v>90.0</v>
+        <v>82.0</v>
       </c>
       <c r="E60" t="n">
         <v>0.0</v>
       </c>
       <c r="F60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G60" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1555,18 +1699,21 @@
         <v>66</v>
       </c>
       <c r="B61" t="n">
-        <v>55.0</v>
+        <v>48.0</v>
       </c>
       <c r="C61" t="n">
-        <v>27.0</v>
+        <v>20.0</v>
       </c>
       <c r="D61" t="n">
-        <v>96.0</v>
+        <v>86.0</v>
       </c>
       <c r="E61" t="n">
         <v>0.0</v>
       </c>
       <c r="F61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G61" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1575,18 +1722,21 @@
         <v>67</v>
       </c>
       <c r="B62" t="n">
-        <v>42.0</v>
+        <v>45.0</v>
       </c>
       <c r="C62" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="D62" t="n">
-        <v>93.0</v>
+        <v>86.0</v>
       </c>
       <c r="E62" t="n">
         <v>0.0</v>
       </c>
       <c r="F62" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G62" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1595,18 +1745,21 @@
         <v>68</v>
       </c>
       <c r="B63" t="n">
-        <v>31.0</v>
+        <v>34.0</v>
       </c>
       <c r="C63" t="n">
-        <v>27.0</v>
+        <v>29.0</v>
       </c>
       <c r="D63" t="n">
-        <v>86.0</v>
+        <v>75.0</v>
       </c>
       <c r="E63" t="n">
         <v>0.0</v>
       </c>
       <c r="F63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G63" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1618,15 +1771,18 @@
         <v>33.0</v>
       </c>
       <c r="C64" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="D64" t="n">
-        <v>89.0</v>
+        <v>81.0</v>
       </c>
       <c r="E64" t="n">
         <v>0.0</v>
       </c>
       <c r="F64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G64" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1635,18 +1791,21 @@
         <v>70</v>
       </c>
       <c r="B65" t="n">
-        <v>38.0</v>
+        <v>43.0</v>
       </c>
       <c r="C65" t="n">
-        <v>19.0</v>
+        <v>22.0</v>
       </c>
       <c r="D65" t="n">
-        <v>97.0</v>
+        <v>86.0</v>
       </c>
       <c r="E65" t="n">
         <v>0.0</v>
       </c>
       <c r="F65" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G65" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1655,18 +1814,21 @@
         <v>71</v>
       </c>
       <c r="B66" t="n">
-        <v>43.0</v>
+        <v>44.0</v>
       </c>
       <c r="C66" t="n">
-        <v>23.0</v>
+        <v>26.0</v>
       </c>
       <c r="D66" t="n">
-        <v>100.0</v>
+        <v>96.0</v>
       </c>
       <c r="E66" t="n">
         <v>0.0</v>
       </c>
       <c r="F66" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G66" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1678,15 +1840,18 @@
         <v>40.0</v>
       </c>
       <c r="C67" t="n">
-        <v>22.0</v>
+        <v>26.0</v>
       </c>
       <c r="D67" t="n">
-        <v>85.0</v>
+        <v>86.0</v>
       </c>
       <c r="E67" t="n">
         <v>0.0</v>
       </c>
       <c r="F67" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G67" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1695,18 +1860,21 @@
         <v>73</v>
       </c>
       <c r="B68" t="n">
-        <v>45.0</v>
+        <v>42.0</v>
       </c>
       <c r="C68" t="n">
         <v>22.0</v>
       </c>
       <c r="D68" t="n">
-        <v>90.0</v>
+        <v>100.0</v>
       </c>
       <c r="E68" t="n">
         <v>0.0</v>
       </c>
       <c r="F68" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G68" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1715,18 +1883,21 @@
         <v>74</v>
       </c>
       <c r="B69" t="n">
-        <v>45.0</v>
+        <v>42.0</v>
       </c>
       <c r="C69" t="n">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
       <c r="D69" t="n">
-        <v>82.0</v>
+        <v>88.0</v>
       </c>
       <c r="E69" t="n">
         <v>0.0</v>
       </c>
       <c r="F69" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G69" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1738,15 +1909,18 @@
         <v>32.0</v>
       </c>
       <c r="C70" t="n">
-        <v>25.0</v>
+        <v>28.0</v>
       </c>
       <c r="D70" t="n">
-        <v>76.0</v>
+        <v>78.0</v>
       </c>
       <c r="E70" t="n">
         <v>0.0</v>
       </c>
       <c r="F70" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G70" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1755,18 +1929,21 @@
         <v>76</v>
       </c>
       <c r="B71" t="n">
-        <v>38.0</v>
+        <v>37.0</v>
       </c>
       <c r="C71" t="n">
-        <v>31.0</v>
+        <v>30.0</v>
       </c>
       <c r="D71" t="n">
-        <v>90.0</v>
+        <v>92.0</v>
       </c>
       <c r="E71" t="n">
         <v>0.0</v>
       </c>
       <c r="F71" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G71" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1775,18 +1952,21 @@
         <v>77</v>
       </c>
       <c r="B72" t="n">
-        <v>43.0</v>
+        <v>46.0</v>
       </c>
       <c r="C72" t="n">
         <v>25.0</v>
       </c>
       <c r="D72" t="n">
-        <v>96.0</v>
+        <v>93.0</v>
       </c>
       <c r="E72" t="n">
         <v>0.0</v>
       </c>
       <c r="F72" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G72" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1795,18 +1975,21 @@
         <v>78</v>
       </c>
       <c r="B73" t="n">
-        <v>46.0</v>
+        <v>50.0</v>
       </c>
       <c r="C73" t="n">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="D73" t="n">
-        <v>83.0</v>
+        <v>88.0</v>
       </c>
       <c r="E73" t="n">
         <v>0.0</v>
       </c>
       <c r="F73" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G73" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1815,18 +1998,21 @@
         <v>79</v>
       </c>
       <c r="B74" t="n">
-        <v>45.0</v>
+        <v>48.0</v>
       </c>
       <c r="C74" t="n">
         <v>24.0</v>
       </c>
       <c r="D74" t="n">
-        <v>86.0</v>
+        <v>92.0</v>
       </c>
       <c r="E74" t="n">
         <v>0.0</v>
       </c>
       <c r="F74" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G74" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1835,18 +2021,21 @@
         <v>80</v>
       </c>
       <c r="B75" t="n">
-        <v>47.0</v>
+        <v>45.0</v>
       </c>
       <c r="C75" t="n">
-        <v>23.0</v>
+        <v>21.0</v>
       </c>
       <c r="D75" t="n">
-        <v>88.0</v>
+        <v>91.0</v>
       </c>
       <c r="E75" t="n">
         <v>0.0</v>
       </c>
       <c r="F75" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G75" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1855,18 +2044,21 @@
         <v>81</v>
       </c>
       <c r="B76" t="n">
-        <v>39.0</v>
+        <v>38.0</v>
       </c>
       <c r="C76" t="n">
         <v>30.0</v>
       </c>
       <c r="D76" t="n">
-        <v>93.0</v>
+        <v>84.0</v>
       </c>
       <c r="E76" t="n">
         <v>0.0</v>
       </c>
       <c r="F76" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G76" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1881,12 +2073,15 @@
         <v>26.0</v>
       </c>
       <c r="D77" t="n">
-        <v>90.0</v>
+        <v>81.0</v>
       </c>
       <c r="E77" t="n">
         <v>0.0</v>
       </c>
       <c r="F77" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G77" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1895,18 +2090,21 @@
         <v>83</v>
       </c>
       <c r="B78" t="n">
-        <v>35.0</v>
+        <v>43.0</v>
       </c>
       <c r="C78" t="n">
         <v>29.0</v>
       </c>
       <c r="D78" t="n">
-        <v>90.0</v>
+        <v>88.0</v>
       </c>
       <c r="E78" t="n">
         <v>0.0</v>
       </c>
       <c r="F78" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G78" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1915,18 +2113,21 @@
         <v>84</v>
       </c>
       <c r="B79" t="n">
-        <v>42.0</v>
+        <v>47.0</v>
       </c>
       <c r="C79" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="D79" t="n">
-        <v>91.0</v>
+        <v>89.0</v>
       </c>
       <c r="E79" t="n">
         <v>0.0</v>
       </c>
       <c r="F79" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G79" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1935,18 +2136,21 @@
         <v>85</v>
       </c>
       <c r="B80" t="n">
-        <v>42.0</v>
+        <v>50.0</v>
       </c>
       <c r="C80" t="n">
-        <v>26.0</v>
+        <v>29.0</v>
       </c>
       <c r="D80" t="n">
-        <v>87.0</v>
+        <v>82.0</v>
       </c>
       <c r="E80" t="n">
         <v>0.0</v>
       </c>
       <c r="F80" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G80" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1955,18 +2159,21 @@
         <v>86</v>
       </c>
       <c r="B81" t="n">
-        <v>43.0</v>
+        <v>44.0</v>
       </c>
       <c r="C81" t="n">
-        <v>22.0</v>
+        <v>20.0</v>
       </c>
       <c r="D81" t="n">
-        <v>95.0</v>
+        <v>91.0</v>
       </c>
       <c r="E81" t="n">
         <v>0.0</v>
       </c>
       <c r="F81" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G81" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1975,18 +2182,21 @@
         <v>87</v>
       </c>
       <c r="B82" t="n">
-        <v>42.0</v>
+        <v>38.0</v>
       </c>
       <c r="C82" t="n">
         <v>26.0</v>
       </c>
       <c r="D82" t="n">
-        <v>91.0</v>
+        <v>87.0</v>
       </c>
       <c r="E82" t="n">
         <v>0.0</v>
       </c>
       <c r="F82" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G82" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1995,18 +2205,21 @@
         <v>88</v>
       </c>
       <c r="B83" t="n">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="C83" t="n">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
       <c r="D83" t="n">
-        <v>83.0</v>
+        <v>84.0</v>
       </c>
       <c r="E83" t="n">
         <v>0.0</v>
       </c>
       <c r="F83" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G83" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2015,18 +2228,21 @@
         <v>89</v>
       </c>
       <c r="B84" t="n">
-        <v>31.0</v>
+        <v>34.0</v>
       </c>
       <c r="C84" t="n">
-        <v>29.0</v>
+        <v>25.0</v>
       </c>
       <c r="D84" t="n">
-        <v>85.0</v>
+        <v>86.0</v>
       </c>
       <c r="E84" t="n">
         <v>0.0</v>
       </c>
       <c r="F84" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G84" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2035,13 +2251,13 @@
         <v>90</v>
       </c>
       <c r="B85" t="n">
-        <v>40.0</v>
+        <v>48.0</v>
       </c>
       <c r="C85" t="n">
-        <v>30.0</v>
+        <v>28.0</v>
       </c>
       <c r="D85" t="n">
-        <v>81.0</v>
+        <v>87.0</v>
       </c>
       <c r="E85" t="n">
         <v>0.0</v>
@@ -2050,7 +2266,7 @@
         <v>0.0</v>
       </c>
       <c r="G85" t="n">
-        <v>100.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="86">
@@ -2058,13 +2274,13 @@
         <v>91</v>
       </c>
       <c r="B86" t="n">
-        <v>46.0</v>
+        <v>45.0</v>
       </c>
       <c r="C86" t="n">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
       <c r="D86" t="n">
-        <v>82.0</v>
+        <v>89.0</v>
       </c>
       <c r="E86" t="n">
         <v>0.0</v>
@@ -2078,13 +2294,13 @@
         <v>92</v>
       </c>
       <c r="B87" t="n">
-        <v>40.0</v>
+        <v>41.0</v>
       </c>
       <c r="C87" t="n">
-        <v>27.0</v>
+        <v>21.0</v>
       </c>
       <c r="D87" t="n">
-        <v>78.0</v>
+        <v>84.0</v>
       </c>
       <c r="E87" t="n">
         <v>0.0</v>
@@ -2101,10 +2317,10 @@
         <v>42.0</v>
       </c>
       <c r="C88" t="n">
-        <v>26.0</v>
+        <v>30.0</v>
       </c>
       <c r="D88" t="n">
-        <v>89.0</v>
+        <v>92.0</v>
       </c>
       <c r="E88" t="n">
         <v>0.0</v>
@@ -2118,13 +2334,13 @@
         <v>94</v>
       </c>
       <c r="B89" t="n">
-        <v>49.0</v>
+        <v>46.0</v>
       </c>
       <c r="C89" t="n">
-        <v>34.0</v>
+        <v>26.0</v>
       </c>
       <c r="D89" t="n">
-        <v>93.0</v>
+        <v>92.0</v>
       </c>
       <c r="E89" t="n">
         <v>0.0</v>
@@ -2138,13 +2354,13 @@
         <v>95</v>
       </c>
       <c r="B90" t="n">
-        <v>50.0</v>
+        <v>52.0</v>
       </c>
       <c r="C90" t="n">
-        <v>23.0</v>
+        <v>28.0</v>
       </c>
       <c r="D90" t="n">
-        <v>86.0</v>
+        <v>83.0</v>
       </c>
       <c r="E90" t="n">
         <v>0.0</v>
@@ -2158,13 +2374,13 @@
         <v>96</v>
       </c>
       <c r="B91" t="n">
-        <v>34.0</v>
+        <v>41.0</v>
       </c>
       <c r="C91" t="n">
-        <v>28.0</v>
+        <v>26.0</v>
       </c>
       <c r="D91" t="n">
-        <v>73.0</v>
+        <v>77.0</v>
       </c>
       <c r="E91" t="n">
         <v>0.0</v>
@@ -2178,13 +2394,13 @@
         <v>97</v>
       </c>
       <c r="B92" t="n">
-        <v>49.0</v>
+        <v>41.0</v>
       </c>
       <c r="C92" t="n">
-        <v>26.0</v>
+        <v>24.0</v>
       </c>
       <c r="D92" t="n">
-        <v>70.0</v>
+        <v>76.0</v>
       </c>
       <c r="E92" t="n">
         <v>0.0</v>

</xml_diff>